<commit_message>
Added POST for customer
</commit_message>
<xml_diff>
--- a/dataFiles/CustomerData.xlsx
+++ b/dataFiles/CustomerData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/apiTesting_challenge/dataFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEBFAA2-A5FE-AB45-8FCF-BD39A7606A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47BDDFB-E7AB-F446-BBE1-AB41F0244564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{141FC98E-6DB1-9A46-8C80-630429BF8D0B}"/>
+    <workbookView xWindow="-32660" yWindow="460" windowWidth="32660" windowHeight="20540" xr2:uid="{141FC98E-6DB1-9A46-8C80-630429BF8D0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>email</t>
   </si>
@@ -108,6 +108,21 @@
   </si>
   <si>
     <t>+12233445566</t>
+  </si>
+  <si>
+    <t>npeart@mail.com</t>
+  </si>
+  <si>
+    <t>Neil</t>
+  </si>
+  <si>
+    <t>Peart</t>
+  </si>
+  <si>
+    <t>npeart</t>
+  </si>
+  <si>
+    <t>npeart123</t>
   </si>
 </sst>
 </file>
@@ -460,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0954E494-DE86-7347-B531-EF024E04EF23}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,6 +515,23 @@
       </c>
       <c r="E2" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a customer PUT method for billing addresss
</commit_message>
<xml_diff>
--- a/dataFiles/CustomerData.xlsx
+++ b/dataFiles/CustomerData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/apiTesting_challenge/dataFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47BDDFB-E7AB-F446-BBE1-AB41F0244564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4468315F-1A37-8740-985C-331DD770FBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32660" yWindow="460" windowWidth="32660" windowHeight="20540" xr2:uid="{141FC98E-6DB1-9A46-8C80-630429BF8D0B}"/>
+    <workbookView xWindow="-32660" yWindow="460" windowWidth="32660" windowHeight="20540" activeTab="1" xr2:uid="{141FC98E-6DB1-9A46-8C80-630429BF8D0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>email</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>npeart123</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -477,7 +480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0954E494-DE86-7347-B531-EF024E04EF23}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -541,84 +544,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A654EF-E738-EF45-9F68-AF93F1F7392E}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K2"/>
+    <sheetView tabSelected="1" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>0</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>155</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>306</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>33122</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor test endpoint for customer put over billing address
</commit_message>
<xml_diff>
--- a/dataFiles/CustomerData.xlsx
+++ b/dataFiles/CustomerData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/apiTesting_challenge/dataFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4468315F-1A37-8740-985C-331DD770FBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09D3857-899E-4E4B-8899-79A1B6694E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32660" yWindow="460" windowWidth="32660" windowHeight="20540" activeTab="1" xr2:uid="{141FC98E-6DB1-9A46-8C80-630429BF8D0B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>email</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>1 Aeropost Way</t>
   </si>
 </sst>
 </file>
@@ -547,7 +550,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,7 +610,7 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F2">
         <v>306</v>

</xml_diff>

<commit_message>
Added patch for shipping address on customer endpoint
</commit_message>
<xml_diff>
--- a/dataFiles/CustomerData.xlsx
+++ b/dataFiles/CustomerData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/apiTesting_challenge/dataFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09D3857-899E-4E4B-8899-79A1B6694E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09A1EFC-D1E9-5147-8557-64743EB2D45D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32660" yWindow="460" windowWidth="32660" windowHeight="20540" activeTab="1" xr2:uid="{141FC98E-6DB1-9A46-8C80-630429BF8D0B}"/>
+    <workbookView xWindow="41280" yWindow="760" windowWidth="32660" windowHeight="20540" activeTab="2" xr2:uid="{141FC98E-6DB1-9A46-8C80-630429BF8D0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>email</t>
   </si>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A654EF-E738-EF45-9F68-AF93F1F7392E}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,72 +641,77 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F08C797-93FD-F041-8420-2C75CE0EF016}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView zoomScale="188" zoomScaleNormal="188" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="188" zoomScaleNormal="188" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>155</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>306</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="H2">
-        <v>33122</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="I2">
+        <v>33121</v>
+      </c>
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added a test for pu method on Product description
</commit_message>
<xml_diff>
--- a/dataFiles/CustomerData.xlsx
+++ b/dataFiles/CustomerData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/apiTesting_challenge/dataFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09A1EFC-D1E9-5147-8557-64743EB2D45D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8DADA8-EBB6-DE44-9199-0E775727B5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41280" yWindow="760" windowWidth="32660" windowHeight="20540" activeTab="2" xr2:uid="{141FC98E-6DB1-9A46-8C80-630429BF8D0B}"/>
+    <workbookView xWindow="41280" yWindow="760" windowWidth="32660" windowHeight="20540" activeTab="3" xr2:uid="{141FC98E-6DB1-9A46-8C80-630429BF8D0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
     <sheet name="Billing" sheetId="2" r:id="rId2"/>
     <sheet name="Shipping" sheetId="3" r:id="rId3"/>
+    <sheet name="ProductDesc" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t>email</t>
   </si>
@@ -129,6 +130,24 @@
   </si>
   <si>
     <t>1 Aeropost Way</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Curabitur non nulla sit amet nisl tempus convallis quis ac lectus. Sed porttitor lectus nibh. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Donec velit neque, auctor sit amet aliquam vel, ullamcorper sit amet ligula. Proin eget tortor risus. Cras ultricies ligula sed magna dictum porta. Quisque velit nisi, pretium ut lacinia in, elementum id enim. Vivamus suscipit tortor eget felis porttitor volutpat. Donec rutrum congue leo eget malesuada. Cras ultricies ligula sed magna dictum porta. Nulla quis lorem ut libero malesuada feugiat.</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>V-Neck T-Shirt</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>v-neck-t-shirt</t>
   </si>
 </sst>
 </file>
@@ -643,7 +662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F08C797-93FD-F041-8420-2C75CE0EF016}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="188" zoomScaleNormal="188" workbookViewId="0">
+    <sheetView zoomScale="188" zoomScaleNormal="188" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -716,4 +735,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE76BCDD-0C74-9841-AE96-F9136D912BF6}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>